<commit_message>
Nuovo test su id 32 RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#DAMPSOFTWAREXXX/DAMP_sas/DAMP_-_Volare_FSE_-_LIS_-_RSA/Ver._02.00/accreditamento-checklist_V8.2.1.xlsx
+++ b/GATEWAY/A1#111#DAMPSOFTWAREXXX/DAMP_sas/DAMP_-_Volare_FSE_-_LIS_-_RSA/Ver._02.00/accreditamento-checklist_V8.2.1.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="507">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1948,18 +1948,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2672,234 +2665,230 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+  <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3195,7 +3184,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3265,7 +3254,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4344,10 +4333,10 @@
   <dimension ref="A1:AA809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4393,10 +4382,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="72"/>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="73" t="s">
         <v>503</v>
       </c>
-      <c r="D2" s="81"/>
+      <c r="D2" s="74"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4417,14 +4406,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="76"/>
+      <c r="C3" s="81" t="s">
         <v>504</v>
       </c>
-      <c r="D3" s="81"/>
+      <c r="D3" s="74"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4445,12 +4434,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A4" s="75"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="82" t="s">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="81" t="s">
         <v>505</v>
       </c>
-      <c r="D4" s="81"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4472,12 +4461,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A5" s="77"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79" t="s">
+      <c r="A5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="82" t="s">
         <v>506</v>
       </c>
-      <c r="D5" s="81"/>
+      <c r="D5" s="74"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -5576,10 +5565,10 @@
         <v>66</v>
       </c>
       <c r="F35" s="32">
-        <v>45511</v>
+        <v>45512</v>
       </c>
       <c r="G35" s="33">
-        <v>45511</v>
+        <v>45512</v>
       </c>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -5595,7 +5584,9 @@
       <c r="Q35" s="34"/>
       <c r="R35" s="34"/>
       <c r="S35" s="34"/>
-      <c r="T35" s="34"/>
+      <c r="T35" s="34" t="s">
+        <v>37</v>
+      </c>
       <c r="U35" s="35"/>
       <c r="V35" s="36"/>
       <c r="W35" s="37" t="s">
@@ -17453,7 +17444,7 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -19723,12 +19714,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19990,21 +19984,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20029,18 +20029,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
riaggiornato il file: accreditamento-checklist_V8.2.1.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#DAMPSOFTWAREXXX/DAMP_sas/DAMP_-_Volare_FSE_-_LIS_-_RSA/Ver._02.00/accreditamento-checklist_V8.2.1.xlsx
+++ b/GATEWAY/A1#111#DAMPSOFTWAREXXX/DAMP_sas/DAMP_-_Volare_FSE_-_LIS_-_RSA/Ver._02.00/accreditamento-checklist_V8.2.1.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="507">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1936,6 +1936,9 @@
   </si>
   <si>
     <t>subject_application_version: Ver. 02.00</t>
+  </si>
+  <si>
+    <t>Errore: Il Campo obbligatorio "REFERTO" risulta vuoto.</t>
   </si>
 </sst>
 </file>
@@ -3180,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3260,7 +3263,7 @@
   <dimension ref="A1:B996"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4330,10 +4333,10 @@
   <dimension ref="A1:Y809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5574,13 +5577,27 @@
       </c>
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="34"/>
+      <c r="M35" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="N35" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="O35" s="34" t="s">
+        <v>506</v>
+      </c>
+      <c r="P35" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q35" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="R35" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="S35" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="T35" s="34" t="s">
         <v>67</v>
       </c>
@@ -19532,15 +19549,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19802,27 +19816,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19847,9 +19855,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>